<commit_message>
Tested on my laptop
</commit_message>
<xml_diff>
--- a/test_results/tables_and_charts.xlsx
+++ b/test_results/tables_and_charts.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windy\projects\GitHub\Project3-CUDA-Path-Tracer\test_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Windy\projects\upenn\Project3-CUDA-Path-Tracer\test_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -356,22 +356,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>39.793399999999998</c:v>
+                  <c:v>26.555700000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.571300000000001</c:v>
+                  <c:v>15.0466</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.82043</c:v>
+                  <c:v>3.6853199999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.109900000000003</c:v>
+                  <c:v>29.572299999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6858199999999997</c:v>
+                  <c:v>5.1506699999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9014300000000004</c:v>
+                  <c:v>5.22818</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -592,22 +592,22 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>125.649</c:v>
+                        <c:v>188.28299999999999</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>255.476</c:v>
+                        <c:v>332.30099999999999</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>1037.25</c:v>
+                        <c:v>1356.74</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>118.73699999999999</c:v>
+                        <c:v>169.077</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>747.851</c:v>
+                        <c:v>970.74800000000005</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>724.48699999999997</c:v>
+                        <c:v>956.35599999999999</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1362,10 +1362,10 @@
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1943101</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1687,7 +1687,7 @@
   <dimension ref="A3:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F9" sqref="A3:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,10 +1734,10 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>125.649</v>
+        <v>188.28299999999999</v>
       </c>
       <c r="F4">
-        <v>39.793399999999998</v>
+        <v>26.555700000000002</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1754,10 +1754,10 @@
         <v>9</v>
       </c>
       <c r="E5">
-        <v>255.476</v>
+        <v>332.30099999999999</v>
       </c>
       <c r="F5">
-        <v>19.571300000000001</v>
+        <v>15.0466</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1774,10 +1774,10 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <v>1037.25</v>
+        <v>1356.74</v>
       </c>
       <c r="F6">
-        <v>4.82043</v>
+        <v>3.6853199999999999</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1794,10 +1794,10 @@
         <v>10</v>
       </c>
       <c r="E7">
-        <v>118.73699999999999</v>
+        <v>169.077</v>
       </c>
       <c r="F7">
-        <v>42.109900000000003</v>
+        <v>29.572299999999998</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1814,10 +1814,10 @@
         <v>9</v>
       </c>
       <c r="E8">
-        <v>747.851</v>
+        <v>970.74800000000005</v>
       </c>
       <c r="F8">
-        <v>6.6858199999999997</v>
+        <v>5.1506699999999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,10 +1834,10 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <v>724.48699999999997</v>
+        <v>956.35599999999999</v>
       </c>
       <c r="F9">
-        <v>6.9014300000000004</v>
+        <v>5.22818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sort paths by sorting indices then reshuffle instead of sorting in place
</commit_message>
<xml_diff>
--- a/test_results/tables_and_charts.xlsx
+++ b/test_results/tables_and_charts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>000</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Time for 5000 iterations (s)</t>
+  </si>
+  <si>
+    <t>110* - sort indices and shuffle</t>
   </si>
 </sst>
 </file>
@@ -1357,14 +1360,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1504950</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:colOff>1724025</xdr:colOff>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1943101</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1684,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F9"/>
+  <dimension ref="A3:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F9" sqref="A3:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,6 +1843,26 @@
         <v>5.22818</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>510.15899999999999</v>
+      </c>
+      <c r="F10">
+        <v>9.8008699999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Additional Test: Access Structs in Global Memory vs Copy to Local Memory First
</commit_message>
<xml_diff>
--- a/test_results/tables_and_charts.xlsx
+++ b/test_results/tables_and_charts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>000</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>110* - sort indices and shuffle</t>
+  </si>
+  <si>
+    <t>000** - copy structs to local memory first</t>
   </si>
 </sst>
 </file>
@@ -1206,6 +1209,521 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.28481304636633231"/>
+          <c:y val="3.1983976301015911E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iterations per second</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$4:$A$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$A$4,Sheet1!$A$11)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>000** - copy structs to local memory first</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$4:$F$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$F$4,Sheet1!$F$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>26.555700000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.2193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7814-4E53-89DA-2FE5B8E51FB1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="444"/>
+        <c:overlap val="-90"/>
+        <c:axId val="1931156911"/>
+        <c:axId val="1931161071"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Time for 5000 iterations (s)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="50000"/>
+                              <a:lumOff val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$A$4:$A$11</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Sheet1!$A$4,Sheet1!$A$11)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>000</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>000** - copy structs to local memory first</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$E$4:$E$11</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Sheet1!$E$4,Sheet1!$E$11)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>188.28299999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>171.12</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-7814-4E53-89DA-2FE5B8E51FB1}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1931156911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1931161071"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1931161071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1931156911"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18323991759094632"/>
+          <c:y val="0.11942929631840622"/>
+          <c:w val="0.2759270051873437"/>
+          <c:h val="5.8366159316406173E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1286,6 +1804,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
   <cs:axisTitle>
@@ -1811,6 +2369,530 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2393,6 +3475,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1581151</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>52388</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2698,10 +3812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F10"/>
+  <dimension ref="A3:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2874,6 +3988,26 @@
         <v>9.8008699999999997</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>171.12</v>
+      </c>
+      <c r="F11">
+        <v>29.2193</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
additional optimization by performance freak
</commit_message>
<xml_diff>
--- a/test_results/tables_and_charts.xlsx
+++ b/test_results/tables_and_charts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>000</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>000** - copy structs to local memory first</t>
+  </si>
+  <si>
+    <t>100*** - compact index array instead of `PathSegments` array</t>
   </si>
 </sst>
 </file>
@@ -1245,6 +1248,540 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iterations per second</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$4:$A$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$A$4,Sheet1!$A$11)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>000** - copy structs to local memory first</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$4:$F$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$F$4,Sheet1!$F$11)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>26.555700000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.2193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7814-4E53-89DA-2FE5B8E51FB1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1931156911"/>
+        <c:axId val="1931161071"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Time for 5000 iterations (s)</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$A$4:$A$11</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Sheet1!$A$4,Sheet1!$A$11)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>000</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>000** - copy structs to local memory first</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Sheet1!$E$4:$E$11</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Sheet1!$E$4,Sheet1!$E$11)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>188.28299999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>171.12</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-7814-4E53-89DA-2FE5B8E51FB1}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1931156911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1931161071"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1931161071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1931156911"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.24288425047438331"/>
+          <c:y val="3.1984002961668305E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -1354,18 +1891,21 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$4:$A$11</c15:sqref>
+                    <c15:sqref>Sheet1!$A$4:$A$12</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$A$4,Sheet1!$A$11)</c:f>
+              <c:f>(Sheet1!$A$4:$A$5,Sheet1!$A$12)</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>000** - copy structs to local memory first</c:v>
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100*** - compact index array instead of `PathSegments` array</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1375,26 +1915,29 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$F$4:$F$11</c15:sqref>
+                    <c15:sqref>Sheet1!$F$4:$F$12</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Sheet1!$F$4,Sheet1!$F$11)</c:f>
+              <c:f>(Sheet1!$F$4:$F$5,Sheet1!$F$12)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>26.555700000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.2193</c:v>
+                  <c:v>15.0466</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.028599999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7814-4E53-89DA-2FE5B8E51FB1}"/>
+              <c16:uniqueId val="{00000000-9CDF-4F9D-A5EE-6023A4978014}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1506,20 +2049,23 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$A$4:$A$11</c15:sqref>
+                          <c15:sqref>Sheet1!$A$4:$A$12</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$A$4,Sheet1!$A$11)</c15:sqref>
+                          <c15:sqref>(Sheet1!$A$4:$A$5,Sheet1!$A$12)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
                       <c:pt idx="0">
                         <c:v>000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>000** - copy structs to local memory first</c:v>
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>100*** - compact index array instead of `PathSegments` array</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1529,28 +2075,31 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Sheet1!$E$4:$E$11</c15:sqref>
+                          <c15:sqref>Sheet1!$E$4:$E$12</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Sheet1!$E$4,Sheet1!$E$11)</c15:sqref>
+                          <c15:sqref>(Sheet1!$E$4:$E$5,Sheet1!$E$12)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
                       <c:pt idx="0">
                         <c:v>188.28299999999999</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>171.12</c:v>
+                        <c:v>332.30099999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>156.11000000000001</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-7814-4E53-89DA-2FE5B8E51FB1}"/>
+                    <c16:uniqueId val="{00000001-9CDF-4F9D-A5EE-6023A4978014}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1844,6 +2393,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
   <cs:axisTitle>
@@ -2893,6 +3482,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3507,6 +4599,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3812,10 +4936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F11"/>
+  <dimension ref="A3:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4008,6 +5132,26 @@
         <v>29.2193</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>156.11000000000001</v>
+      </c>
+      <c r="F12">
+        <v>32.028599999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>